<commit_message>
Báo Cáo Doanh Thu
</commit_message>
<xml_diff>
--- a/DuLieu.xlsx
+++ b/DuLieu.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huynh\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2C4A28-F22D-4F2B-8868-4513BE239B76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -253,7 +247,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -354,6 +348,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -415,7 +411,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -450,7 +446,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -627,23 +623,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="23.42578125" style="4"/>
+    <col min="1" max="7" width="23.42578125" style="4"/>
+    <col min="8" max="8" width="23.42578125" style="11"/>
+    <col min="9" max="16384" width="23.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -668,7 +666,7 @@
       <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>72</v>
       </c>
       <c r="I1" s="6" t="s">
@@ -697,7 +695,7 @@
       <c r="G2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="10">
         <v>5000</v>
       </c>
       <c r="I2" s="6">
@@ -726,7 +724,7 @@
       <c r="G3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="10">
         <v>7500</v>
       </c>
       <c r="I3" s="6">
@@ -755,7 +753,7 @@
       <c r="G4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="10">
         <v>20000</v>
       </c>
       <c r="I4" s="6">
@@ -784,7 +782,7 @@
       <c r="G5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="10">
         <v>3000</v>
       </c>
       <c r="I5" s="6">
@@ -813,7 +811,7 @@
       <c r="G6" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="10">
         <v>2000</v>
       </c>
       <c r="I6" s="6">
@@ -842,7 +840,7 @@
       <c r="G7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="10">
         <v>12300</v>
       </c>
       <c r="I7" s="6">
@@ -871,7 +869,7 @@
       <c r="G8" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="10">
         <v>6557</v>
       </c>
       <c r="I8" s="6">
@@ -900,7 +898,7 @@
       <c r="G9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="10">
         <v>9000</v>
       </c>
       <c r="I9" s="6">
@@ -929,7 +927,7 @@
       <c r="G10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="10">
         <v>3400</v>
       </c>
       <c r="I10" s="6">
@@ -958,7 +956,7 @@
       <c r="G11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="10">
         <v>44000</v>
       </c>
       <c r="I11" s="6">
@@ -987,7 +985,7 @@
       <c r="G12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="10">
         <v>8003</v>
       </c>
       <c r="I12" s="6">
@@ -1016,7 +1014,7 @@
       <c r="G13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="10">
         <v>45896</v>
       </c>
       <c r="I13" s="6">
@@ -1025,7 +1023,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1" display="https://www.vinmec.com/vi/tin-tuc/thong-tin-suc-khoe/paracetamol-la-gi/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E12" r:id="rId1" display="https://www.vinmec.com/vi/tin-tuc/thong-tin-suc-khoe/paracetamol-la-gi/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1033,7 +1031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>